<commit_message>
Updated team spreadsheet for code review 2
</commit_message>
<xml_diff>
--- a/TeamContributions.xlsx
+++ b/TeamContributions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danfe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danfe\OneDrive\Desktop\Second Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255938A3-46C3-44A3-8F81-0108AE1BF2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B66DD341-8343-4FF4-8F3F-83160FB5FCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4524" yWindow="2112" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -29,26 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>MEMBERS</t>
   </si>
   <si>
-    <t>WEEK 1 TASKS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Github page, setup and built project with JAR, setup dockerfile and Docker in Github actions and create first release. </t>
-  </si>
-  <si>
-    <t>Created the use cases and use case diagrams and started using and creating our github issues. Helped with issues on project build and setup.</t>
-  </si>
-  <si>
-    <t>Created the backlog, user stories, branches, code of conduct and gave out group tasks. Help with issues on project build and setup.</t>
-  </si>
-  <si>
-    <t>SCORE</t>
-  </si>
-  <si>
     <t>Dan Ferguson - 40534169</t>
   </si>
   <si>
@@ -59,6 +44,12 @@
   </si>
   <si>
     <t>Dale Follows - 40606982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEEK 1 </t>
+  </si>
+  <si>
+    <t>WEEK 2</t>
   </si>
 </sst>
 </file>
@@ -210,13 +201,17 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table" displayName="Table" ref="B2:D6" totalsRowShown="0">
   <autoFilter ref="B2:D6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="MEMBERS"/>
-    <tableColumn id="8" xr3:uid="{D53E75A9-F30D-4BCB-8B14-C1FB3BC3C1A3}" name="WEEK 1 TASKS"/>
-    <tableColumn id="10" xr3:uid="{9E8AC0FF-EF32-418F-9DE3-AAA928D283E0}" name="SCORE"/>
+    <tableColumn id="8" xr3:uid="{D53E75A9-F30D-4BCB-8B14-C1FB3BC3C1A3}" name="WEEK 1 "/>
+    <tableColumn id="10" xr3:uid="{9E8AC0FF-EF32-418F-9DE3-AAA928D283E0}" name="WEEK 2"/>
   </tableColumns>
   <tableStyleInfo name="Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -489,14 +484,14 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="82.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -505,18 +500,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
         <v>2</v>
+      </c>
+      <c r="C3">
+        <v>33</v>
       </c>
       <c r="D3">
         <v>33</v>
@@ -524,10 +519,10 @@
     </row>
     <row r="4" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
       </c>
       <c r="D4">
         <v>33</v>
@@ -536,10 +531,10 @@
     </row>
     <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
         <v>3</v>
+      </c>
+      <c r="C5">
+        <v>33</v>
       </c>
       <c r="D5">
         <v>33</v>
@@ -547,7 +542,10 @@
     </row>
     <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>

</xml_diff>